<commit_message>
update job, roadmap, scenario
</commit_message>
<xml_diff>
--- a/project/documentation/scenario.xlsx
+++ b/project/documentation/scenario.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,48 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Захожу в католог</t>
   </si>
   <si>
-    <t>Ввожу в поисковой строке название фильма</t>
-  </si>
-  <si>
-    <t>Выбираю фильм из предложенного списка</t>
-  </si>
-  <si>
-    <t>Попадаю на страницу с описанием фильма</t>
-  </si>
-  <si>
-    <t>Ищу в каталоге интересующий меня фильм</t>
-  </si>
-  <si>
-    <t>Перехожу на страницу с описанием фильма</t>
-  </si>
-  <si>
-    <t>Выбираю понравившийся фильм</t>
-  </si>
-  <si>
-    <t>Выбираю интересующий жанр</t>
-  </si>
-  <si>
-    <t>Перехожу в каталог жанров</t>
-  </si>
-  <si>
-    <t>Перехожу в свой профиль</t>
-  </si>
-  <si>
-    <t>Смотрю просмотренные мной фильмы, оставленные отзывы\оценки</t>
-  </si>
-  <si>
-    <t>Захожу в каталог</t>
-  </si>
-  <si>
-    <t>Перехожу в описание фильма</t>
-  </si>
-  <si>
-    <t>Оставляю отзыв, оценку</t>
+    <t>Ввожу в поисковой строке  что хочешь купить</t>
+  </si>
+  <si>
+    <t>Нажимаешь кнопку поиск</t>
+  </si>
+  <si>
+    <t>переходишь по ссылке и покупаешь вещь</t>
+  </si>
+  <si>
+    <t>Регестрируешься</t>
+  </si>
+  <si>
+    <t>Добавляешь свою необычную вещь/продукт</t>
+  </si>
+  <si>
+    <t>Сортируешь по: отзывам, стоимости, региону, рейтингу, времени прибытия, типу товара</t>
   </si>
 </sst>
 </file>
@@ -153,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,7 +167,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +391,7 @@
     <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,10 +402,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -434,49 +416,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>